<commit_message>
assets: :bento: updated excel header for commodity
</commit_message>
<xml_diff>
--- a/public/import-barang-template.xlsx
+++ b/public/import-barang-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univ\Self\Belajar Laravel\Laravel 6\Project\inventaris\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lenovo\developments\laravel\inven-bs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E38D0E-5BE3-41CA-92A4-E9A26158767C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817B158-F286-473E-93D4-8EA97E50A231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,16 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -30,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>No.</t>
-  </si>
-  <si>
     <t>Kode Barang</t>
   </si>
   <si>
@@ -48,9 +53,6 @@
     <t>Asal Perolehan</t>
   </si>
   <si>
-    <t>Lokasi</t>
-  </si>
-  <si>
     <t>Tahun Pembelian</t>
   </si>
   <si>
@@ -67,6 +69,12 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Lokasi Barang</t>
   </si>
 </sst>
 </file>
@@ -409,65 +417,65 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assets: :bento: updated import excel template on commodity
</commit_message>
<xml_diff>
--- a/public/import-barang-template.xlsx
+++ b/public/import-barang-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lenovo\developments\laravel\inven-bs\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817B158-F286-473E-93D4-8EA97E50A231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817F6859-6151-4E01-A377-4F17062D34F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Kode Barang</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Keterangan</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Lokasi Barang</t>
@@ -414,67 +411,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>